<commit_message>
Review XLSX formulae for conditional formatting
</commit_message>
<xml_diff>
--- a/construct-logic/src/test/resources/org/keyboardplaying/xtt/xlsx/tracker-dev.xlsx
+++ b/construct-logic/src/test/resources/org/keyboardplaying/xtt/xlsx/tracker-dev.xlsx
@@ -715,7 +715,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -751,6 +751,82 @@
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -876,18 +952,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:I16" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:I16" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <tableColumns count="8">
-    <tableColumn id="1" name="Rule set" dataDxfId="18">
+    <tableColumn id="1" name="Rule set" dataDxfId="29">
       <calculatedColumnFormula>ROW() - 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="17"/>
-    <tableColumn id="3" name="Day length" dataDxfId="16"/>
-    <tableColumn id="4" name="Min. pause" dataDxfId="15"/>
-    <tableColumn id="7" name="Arrive before" dataDxfId="14"/>
-    <tableColumn id="5" name="Counted from" dataDxfId="13"/>
-    <tableColumn id="8" name="Leave after" dataDxfId="12"/>
-    <tableColumn id="6" name="Counted to" dataDxfId="11"/>
+    <tableColumn id="2" name="Name" dataDxfId="28"/>
+    <tableColumn id="3" name="Day length" dataDxfId="27"/>
+    <tableColumn id="4" name="Min. pause" dataDxfId="26"/>
+    <tableColumn id="7" name="Arrive before" dataDxfId="25"/>
+    <tableColumn id="5" name="Counted from" dataDxfId="24"/>
+    <tableColumn id="8" name="Leave after" dataDxfId="23"/>
+    <tableColumn id="6" name="Counted to" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1351,11 +1427,11 @@
       <c r="H3" s="12"/>
       <c r="I3" s="10">
         <f ca="1">IF($W3,IF(ISNUMBER($G3),$G3,NOW()-TODAY())-$F3+$E3-$D3-$H3,"")</f>
-        <v>0.89599976851604879</v>
+        <v>0.90804618055699393</v>
       </c>
       <c r="J3" s="4">
         <f ca="1">IF($W3, IF(ISNUMBER($G3), MIN($G3,OFFSET(Cfg!$B$6, $B3, 7)),NOW()-TODAY()) - IF($C3 &gt; Cfg!$F$4, MAX($F3-$E3, OFFSET(Cfg!$B$6, $B3, 3)), $F3 - $E3) - IF(ISNUMBER($D3),MAX($D3,OFFSET(Cfg!$B$6, $B3, 5)),0) - $H3, "")</f>
-        <v>0.89599976851604879</v>
+        <v>0.90804618055699393</v>
       </c>
       <c r="K3" s="29" t="str">
         <f t="shared" ref="K3" ca="1" si="0" xml:space="preserve"> IF(AND($W3, $AC3 &lt; 0), "-", "")</f>
@@ -1363,11 +1439,11 @@
       </c>
       <c r="L3" s="30">
         <f t="shared" ref="L3" ca="1" si="1">IF($W3, ABS($AC3), "")</f>
-        <v>0.56266643518271553</v>
+        <v>0.57471284722366067</v>
       </c>
       <c r="M3" s="10">
         <f ca="1">IF($W3,SUM($J$3:$J3),"")</f>
-        <v>0.89599976851604879</v>
+        <v>0.90804618055699393</v>
       </c>
       <c r="N3" s="4">
         <f ca="1">IF($W3,SUM($Z$3:$Z3),"")</f>
@@ -1379,11 +1455,11 @@
       </c>
       <c r="P3" s="30">
         <f t="shared" ref="P3" ca="1" si="3">IF($W3,ABS($AD3),"")</f>
-        <v>0.56266643518271553</v>
+        <v>0.57471284722366067</v>
       </c>
       <c r="Q3" s="10">
         <f ca="1">IF($W3,SUM($J$3:$J3),"")</f>
-        <v>0.89599976851604879</v>
+        <v>0.90804618055699393</v>
       </c>
       <c r="R3" s="4">
         <f ca="1">IF($W3,SUM($Z$3:$Z3),"")</f>
@@ -1395,7 +1471,7 @@
       </c>
       <c r="T3" s="30">
         <f ca="1">IF($W3, ABS($Q3-$R3), "")</f>
-        <v>0.56266643518271553</v>
+        <v>0.57471284722366067</v>
       </c>
       <c r="U3" s="20">
         <v>1</v>
@@ -1428,11 +1504,11 @@
       </c>
       <c r="AC3" s="42">
         <f ca="1">IF($W3, $J3 - $Z3, "")</f>
-        <v>0.56266643518271553</v>
+        <v>0.57471284722366067</v>
       </c>
       <c r="AD3" s="42">
         <f ca="1">IF($W3, $M3 - $N3, "")</f>
-        <v>0.56266643518271553</v>
+        <v>0.57471284722366067</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1459,7 +1535,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="31">
         <f ca="1">IF(ISNUMBER($B4),SUMIF($B$3:$B3,$B4,$J$3:$J3),SUM($J$3:$J3))</f>
-        <v>0.89599976851604879</v>
+        <v>0.90804618055699393</v>
       </c>
       <c r="N4" s="32">
         <f ca="1">IF(ISNUMBER($B4),SUMIF($B$3:$B3,$B4,$Z$3:$Z3),SUM($Z$3:$Z3))</f>
@@ -1471,11 +1547,11 @@
       </c>
       <c r="P4" s="36">
         <f ca="1">ABS(M4-N4)</f>
-        <v>0.56266643518271553</v>
+        <v>0.57471284722366067</v>
       </c>
       <c r="Q4" s="31">
         <f ca="1">IF(ISNUMBER($B4),SUMIF($B$3:$B3,$B4,$J$3:$J3),SUM($J$3:$J3))</f>
-        <v>0.89599976851604879</v>
+        <v>0.90804618055699393</v>
       </c>
       <c r="R4" s="32">
         <f ca="1">IF(ISNUMBER($B4),SUMIF($B$3:$B3,$B4,$Z$3:$Z3),SUM($Z$3:$Z3))</f>
@@ -1487,7 +1563,7 @@
       </c>
       <c r="T4" s="36">
         <f ca="1">ABS(Q4-R4)</f>
-        <v>0.56266643518271553</v>
+        <v>0.57471284722366067</v>
       </c>
       <c r="U4" s="20">
         <v>1</v>
@@ -1541,52 +1617,52 @@
     <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:L4">
-    <cfRule type="expression" dxfId="10" priority="400">
-      <formula xml:space="preserve"> AND($W3, $K3 = "-")</formula>
+    <cfRule type="expression" dxfId="21" priority="400">
+      <formula>AND($W3, $K3 = "-")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:C4">
-    <cfRule type="expression" dxfId="9" priority="370">
-      <formula xml:space="preserve"> $W3 = FALSE</formula>
+    <cfRule type="expression" dxfId="20" priority="370">
+      <formula>NOT($W3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:T4">
-    <cfRule type="expression" dxfId="8" priority="371" stopIfTrue="1">
-      <formula xml:space="preserve"> $W3 = FALSE</formula>
+    <cfRule type="expression" dxfId="19" priority="371" stopIfTrue="1">
+      <formula>NOT($W3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:T4">
-    <cfRule type="expression" dxfId="7" priority="4">
-      <formula xml:space="preserve"> AND($X3, $S3 = "-")</formula>
+    <cfRule type="expression" dxfId="18" priority="4">
+      <formula>AND($X3, $S3 = "-")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="401">
-      <formula xml:space="preserve"> AND($W3, $S3 = "-")</formula>
+    <cfRule type="expression" dxfId="17" priority="401">
+      <formula>AND($W3, $S3 = "-")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:T4">
-    <cfRule type="expression" dxfId="5" priority="365" stopIfTrue="1">
-      <formula xml:space="preserve"> $X3</formula>
+    <cfRule type="expression" dxfId="11" priority="365" stopIfTrue="1">
+      <formula>$X3 = TRUE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="403">
-      <formula xml:space="preserve"> $A3 = TODAY()</formula>
+    <cfRule type="expression" dxfId="16" priority="403">
+      <formula>$A3 = TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:P4">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula xml:space="preserve"> AND($X3, $O3 = "-")</formula>
+    <cfRule type="expression" dxfId="15" priority="3">
+      <formula>AND($X3, $O3 = "-")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="402">
-      <formula xml:space="preserve"> AND($W3, $O3 = "-")</formula>
+    <cfRule type="expression" dxfId="14" priority="402">
+      <formula>AND($W3, $O3 = "-")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D4">
-    <cfRule type="expression" dxfId="1" priority="399">
-      <formula xml:space="preserve"> AND($AA3, $D3, $D3 &gt; $AA3)</formula>
+    <cfRule type="expression" dxfId="13" priority="399">
+      <formula>AND($AA3, $D3, $D3 &gt; $AA3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="expression" dxfId="0" priority="398">
-      <formula xml:space="preserve"> AND($AB3, $G3, $G3 &lt; $AB3)</formula>
+    <cfRule type="expression" dxfId="12" priority="398">
+      <formula>AND($AB3, $G3, $G3 &lt; $AB3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC3:AC4">

</xml_diff>